<commit_message>
update layer1 layer2 testing
</commit_message>
<xml_diff>
--- a/test_sheet.xlsx
+++ b/test_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12CF5B6-627D-44F2-9D70-CEC4F798EA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A4F2F2-416D-4399-BCDC-AF64E64ECD99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="199">
   <si>
     <t>formatId</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -622,10 +622,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数据检查</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -757,6 +753,41 @@
   </si>
   <si>
     <t>SS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>级别二测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>质量块级别二测试需要检查质量块数量与实际质量块是否相符，如质量块数量为3，则质量块必须有3个。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表示 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表示数量级别二测试需要检查表示数量（本字段的数量）与实际的表示是否相符，表示数量为1，则表示必须有1个。（表示实际就是附录B.2 中的Body）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>级别一测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>representationBody1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -834,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -854,6 +885,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,23 +1169,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.44140625" customWidth="1"/>
     <col min="4" max="4" width="50.109375" customWidth="1"/>
-    <col min="5" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" customWidth="1"/>
-    <col min="8" max="9" width="33.77734375" customWidth="1"/>
-    <col min="10" max="10" width="37.21875" customWidth="1"/>
+    <col min="5" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" customWidth="1"/>
+    <col min="9" max="10" width="33.77734375" customWidth="1"/>
+    <col min="11" max="11" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>106</v>
       </c>
@@ -1165,25 +1199,28 @@
         <v>155</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="F1" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" t="s">
         <v>114</v>
       </c>
-      <c r="H1" t="s">
-        <v>159</v>
-      </c>
       <c r="I1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1197,23 +1234,23 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G2" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" t="s">
         <v>189</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1226,18 +1263,18 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1251,16 +1288,19 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G4" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1274,19 +1314,25 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1300,1393 +1346,1414 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>195</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="G8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>148</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" s="4"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="3"/>
+      <c r="K9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F10" t="s">
-        <v>175</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F11" t="s">
-        <v>175</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G11" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F12" t="s">
-        <v>175</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G12" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" t="s">
-        <v>175</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G13" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>157</v>
-      </c>
-      <c r="F14" t="s">
-        <v>175</v>
-      </c>
-      <c r="G14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F15" t="s">
-        <v>175</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G15" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" t="s">
-        <v>177</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E17" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" t="s">
-        <v>175</v>
-      </c>
-      <c r="G18" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G18" t="s">
+        <v>174</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
-      </c>
-      <c r="F19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="E19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G19" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="J20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="G20" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="K20" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="K21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" t="s">
-        <v>157</v>
-      </c>
-      <c r="F22" t="s">
-        <v>180</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="H22">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E23" t="s">
-        <v>157</v>
-      </c>
-      <c r="F23" t="s">
-        <v>175</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H23">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G23" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F24" t="s">
-        <v>175</v>
-      </c>
-      <c r="G24" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" t="s">
+        <v>174</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H24">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>83</v>
-      </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" t="s">
-        <v>180</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="H26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>157</v>
-      </c>
-      <c r="F27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H27">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G27" t="s">
+        <v>179</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" t="s">
+        <v>174</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H28">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="E29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" t="s">
+        <v>174</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" t="s">
-        <v>157</v>
-      </c>
-      <c r="F30" t="s">
-        <v>180</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="H30">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H31">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I31">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F32" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" t="s">
+        <v>174</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H32">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
-      </c>
-      <c r="F33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G33" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>86</v>
-      </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" t="s">
-        <v>181</v>
-      </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
       <c r="C35" t="s">
-        <v>183</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>182</v>
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>180</v>
       </c>
       <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="D36" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" t="s">
-        <v>157</v>
-      </c>
-      <c r="F36" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H36">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>182</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s">
-        <v>157</v>
-      </c>
-      <c r="F37" t="s">
-        <v>175</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H37">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G37" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I37">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" t="s">
-        <v>32</v>
-      </c>
       <c r="D38" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" t="s">
-        <v>181</v>
-      </c>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G38" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I38">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
       <c r="C39" t="s">
-        <v>183</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>182</v>
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" t="s">
+        <v>180</v>
       </c>
       <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="D40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" t="s">
-        <v>157</v>
-      </c>
-      <c r="F40" t="s">
-        <v>175</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H40">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>182</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H41">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G41" t="s">
+        <v>174</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" t="s">
-        <v>33</v>
-      </c>
       <c r="D42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F42" t="s">
-        <v>181</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E42" t="s">
+        <v>156</v>
+      </c>
+      <c r="G42" t="s">
+        <v>174</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I42">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
       <c r="C43" t="s">
-        <v>183</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>182</v>
+        <v>33</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+      <c r="G43" t="s">
+        <v>180</v>
       </c>
       <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="D44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" t="s">
-        <v>157</v>
-      </c>
-      <c r="F44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H44">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>182</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E45" t="s">
-        <v>157</v>
-      </c>
-      <c r="F45" t="s">
-        <v>175</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H45">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G45" t="s">
+        <v>174</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I45">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
       <c r="D46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" t="s">
-        <v>181</v>
-      </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E46" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I46">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
       <c r="C47" t="s">
-        <v>183</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>182</v>
+        <v>34</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" t="s">
+        <v>180</v>
       </c>
       <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="D48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" t="s">
-        <v>157</v>
-      </c>
-      <c r="F48" t="s">
-        <v>175</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H48">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>182</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" t="s">
-        <v>175</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H49">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I49">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>90</v>
-      </c>
-      <c r="C50" t="s">
-        <v>42</v>
-      </c>
       <c r="D50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E50" t="s">
-        <v>157</v>
-      </c>
-      <c r="F50" t="s">
-        <v>175</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G50" t="s">
+        <v>174</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I50">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E51" t="s">
-        <v>157</v>
-      </c>
-      <c r="F51" t="s">
-        <v>175</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="H51" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G51" t="s">
+        <v>174</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D52" t="s">
-        <v>167</v>
+        <v>43</v>
       </c>
       <c r="E52" t="s">
-        <v>157</v>
-      </c>
-      <c r="F52" t="s">
-        <v>175</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H52">
-        <v>-111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G52" t="s">
+        <v>174</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="E53" t="s">
-        <v>157</v>
-      </c>
-      <c r="F53" t="s">
-        <v>175</v>
-      </c>
-      <c r="G53" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G53" t="s">
+        <v>174</v>
+      </c>
+      <c r="H53" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H53">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>-111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>47</v>
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
+        <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E54" t="s">
-        <v>157</v>
-      </c>
-      <c r="F54" t="s">
-        <v>175</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H54">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G54" t="s">
+        <v>174</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I54">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" t="s">
-        <v>48</v>
+        <v>94</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
-      </c>
-      <c r="F55" t="s">
-        <v>175</v>
-      </c>
-      <c r="G55" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G55" t="s">
+        <v>174</v>
+      </c>
+      <c r="H55" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H55">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="I55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>170</v>
+        <v>52</v>
       </c>
       <c r="E56" t="s">
-        <v>157</v>
-      </c>
-      <c r="F56" t="s">
-        <v>175</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H56">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G56" t="s">
+        <v>174</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I56">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D57" t="s">
         <v>169</v>
       </c>
       <c r="E57" t="s">
-        <v>157</v>
-      </c>
-      <c r="F57" t="s">
-        <v>175</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H57">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G57" t="s">
+        <v>174</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I57">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
+        <v>53</v>
+      </c>
       <c r="D58" t="s">
-        <v>60</v>
-      </c>
-      <c r="F58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="E58" t="s">
+        <v>156</v>
+      </c>
+      <c r="G58" t="s">
+        <v>174</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I58">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
-        <v>183</v>
-      </c>
-      <c r="H59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>60</v>
+      </c>
+      <c r="G59" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>98</v>
-      </c>
       <c r="C60" t="s">
-        <v>57</v>
-      </c>
-      <c r="D60" t="s">
-        <v>54</v>
-      </c>
-      <c r="E60" t="s">
-        <v>157</v>
-      </c>
-      <c r="F60" t="s">
-        <v>175</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H60">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="I60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E61" t="s">
-        <v>157</v>
-      </c>
-      <c r="F61" t="s">
-        <v>175</v>
-      </c>
-      <c r="G61" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G61" t="s">
+        <v>174</v>
+      </c>
+      <c r="H61" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H61">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E62" t="s">
-        <v>157</v>
-      </c>
-      <c r="F62" t="s">
-        <v>175</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H62">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="G62" t="s">
+        <v>174</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" t="s">
+        <v>59</v>
+      </c>
       <c r="D63" t="s">
-        <v>168</v>
-      </c>
-      <c r="F63" t="s">
-        <v>181</v>
-      </c>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E63" t="s">
+        <v>156</v>
+      </c>
+      <c r="G63" t="s">
+        <v>174</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I63">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="C64" t="s">
-        <v>183</v>
-      </c>
-      <c r="G64" s="7"/>
-      <c r="H64">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>167</v>
+      </c>
+      <c r="G64" t="s">
+        <v>180</v>
+      </c>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>101</v>
-      </c>
       <c r="C65" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" t="s">
-        <v>61</v>
-      </c>
-      <c r="E65" t="s">
-        <v>157</v>
-      </c>
-      <c r="F65" t="s">
-        <v>175</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H65">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="H65" s="7"/>
+      <c r="I65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E66" t="s">
-        <v>157</v>
-      </c>
-      <c r="F66" t="s">
-        <v>175</v>
-      </c>
-      <c r="G66" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G66" t="s">
+        <v>174</v>
+      </c>
+      <c r="H66" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H66">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E67" t="s">
-        <v>157</v>
-      </c>
-      <c r="F67" t="s">
-        <v>175</v>
-      </c>
-      <c r="G67" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G67" t="s">
+        <v>174</v>
+      </c>
+      <c r="H67" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H67">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E68" t="s">
-        <v>157</v>
-      </c>
-      <c r="F68" t="s">
-        <v>175</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H68">
+        <v>156</v>
+      </c>
+      <c r="G68" t="s">
+        <v>174</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I68">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" t="s">
+        <v>156</v>
+      </c>
+      <c r="G69" t="s">
+        <v>174</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
         <v>105</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>68</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>70</v>
       </c>
-      <c r="F69" t="s">
-        <v>174</v>
-      </c>
-      <c r="H69" s="3" t="s">
+      <c r="G70" t="s">
         <v>173</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>